<commit_message>
Updated to work with dash
</commit_message>
<xml_diff>
--- a/TestAccounts.xlsx
+++ b/TestAccounts.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="14235"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -418,7 +418,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>